<commit_message>
cleaning up all the unnecessary spreadsheets
</commit_message>
<xml_diff>
--- a/Image_Analysis/Archive/tissue_im_test.xlsx
+++ b/Image_Analysis/Archive/tissue_im_test.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tfai/Documents/GitHub/Minimal-Lung-Model/Image_Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tfai/Documents/GitHub/Minimal-Lung-Model/Image_Analysis/Archive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C5BFC0-C6EB-E547-9179-FEF66D3B1DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449A8961-A23E-EE4C-84AD-1F21C3427755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="880" yWindow="500" windowWidth="35840" windowHeight="20380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MLI_new" sheetId="2" r:id="rId1"/>
     <sheet name="MLI_old" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="16">
   <si>
     <t>Animal Number</t>
   </si>
@@ -77,6 +79,9 @@
   <si>
     <t>MLI_edit pics</t>
   </si>
+  <si>
+    <t>ID</t>
+  </si>
 </sst>
 </file>
 
@@ -99,7 +104,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,6 +187,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -361,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -402,21 +419,33 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,7 +471,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -730,7 +759,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -741,14 +770,13 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="C2" sqref="C2:C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10.83203125" style="44"/>
-    <col min="3" max="3" width="10.83203125" style="46"/>
-    <col min="4" max="4" width="10.83203125" style="48"/>
+    <col min="4" max="4" width="10.83203125" style="47"/>
     <col min="5" max="5" width="10.83203125" style="41"/>
   </cols>
   <sheetData>
@@ -779,10 +807,10 @@
       <c r="C2" s="45">
         <v>217</v>
       </c>
-      <c r="D2" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="47">
+      <c r="D2" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="46">
         <v>28.857949839922696</v>
       </c>
     </row>
@@ -1582,8 +1610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4AE4827-4420-E84F-933E-83FF9CDB4E70}">
   <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1611,14 +1639,14 @@
         <v>14</v>
       </c>
       <c r="H1" s="11"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="50"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="49"/>
     </row>
     <row r="2" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="12">
@@ -1627,7 +1655,7 @@
       <c r="B2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="51" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="14" t="s">
@@ -1643,14 +1671,14 @@
         <v>32.109248440000002</v>
       </c>
       <c r="H2" s="11"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
     </row>
     <row r="3" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="18">
@@ -1675,14 +1703,14 @@
         <v>15.89621037</v>
       </c>
       <c r="H3" s="11"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="49"/>
+      <c r="P3" s="49"/>
     </row>
     <row r="4" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="18">
@@ -1707,14 +1735,14 @@
         <v>38.263251840000002</v>
       </c>
       <c r="H4" s="11"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="50"/>
-      <c r="P4" s="50"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="49"/>
+      <c r="P4" s="49"/>
     </row>
     <row r="5" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="18">
@@ -1739,14 +1767,14 @@
         <v>35.393663490000002</v>
       </c>
       <c r="H5" s="11"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="50"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="49"/>
     </row>
     <row r="6" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
@@ -1771,14 +1799,14 @@
         <v>21.516547580000001</v>
       </c>
       <c r="H6" s="11"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="50"/>
-      <c r="N6" s="50"/>
-      <c r="O6" s="50"/>
-      <c r="P6" s="50"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="49"/>
+      <c r="P6" s="49"/>
     </row>
     <row r="7" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
@@ -1803,14 +1831,14 @@
         <v>33.930421510000002</v>
       </c>
       <c r="H7" s="11"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="50"/>
-      <c r="P7" s="50"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="49"/>
+      <c r="P7" s="49"/>
     </row>
     <row r="8" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
@@ -1835,14 +1863,14 @@
         <v>28.414697029999999</v>
       </c>
       <c r="H8" s="11"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="50"/>
-      <c r="L8" s="50"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="50"/>
-      <c r="O8" s="50"/>
-      <c r="P8" s="50"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="49"/>
     </row>
     <row r="9" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
@@ -1867,14 +1895,14 @@
         <v>34.975110540000003</v>
       </c>
       <c r="H9" s="11"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="50"/>
-      <c r="K9" s="50"/>
-      <c r="L9" s="50"/>
-      <c r="M9" s="50"/>
-      <c r="N9" s="50"/>
-      <c r="O9" s="50"/>
-      <c r="P9" s="50"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
+      <c r="N9" s="49"/>
+      <c r="O9" s="49"/>
+      <c r="P9" s="49"/>
     </row>
     <row r="10" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="18">
@@ -1899,14 +1927,14 @@
         <v>21.896100820000001</v>
       </c>
       <c r="H10" s="11"/>
-      <c r="I10" s="50"/>
-      <c r="J10" s="50"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="50"/>
-      <c r="O10" s="50"/>
-      <c r="P10" s="50"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="49"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="49"/>
+      <c r="P10" s="49"/>
     </row>
     <row r="11" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="18">
@@ -1931,14 +1959,14 @@
         <v>37.771244889999998</v>
       </c>
       <c r="H11" s="11"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
-      <c r="L11" s="50"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="50"/>
-      <c r="O11" s="50"/>
-      <c r="P11" s="50"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="49"/>
+      <c r="P11" s="49"/>
     </row>
     <row r="12" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="18">
@@ -1963,14 +1991,14 @@
         <v>39.789910079999999</v>
       </c>
       <c r="H12" s="11"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="50"/>
-      <c r="L12" s="50"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="50"/>
-      <c r="O12" s="50"/>
-      <c r="P12" s="50"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="49"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="49"/>
+      <c r="P12" s="49"/>
     </row>
     <row r="13" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
@@ -1995,14 +2023,14 @@
         <v>36.066911660000002</v>
       </c>
       <c r="H13" s="11"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="50"/>
-      <c r="K13" s="50"/>
-      <c r="L13" s="50"/>
-      <c r="M13" s="50"/>
-      <c r="N13" s="50"/>
-      <c r="O13" s="50"/>
-      <c r="P13" s="50"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="49"/>
+      <c r="M13" s="49"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="49"/>
+      <c r="P13" s="49"/>
     </row>
     <row r="14" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
@@ -2027,14 +2055,14 @@
         <v>14.898635609999999</v>
       </c>
       <c r="H14" s="11"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="50"/>
-      <c r="L14" s="50"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="50"/>
-      <c r="O14" s="50"/>
-      <c r="P14" s="50"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="49"/>
+      <c r="O14" s="49"/>
+      <c r="P14" s="49"/>
     </row>
     <row r="15" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
@@ -2059,14 +2087,14 @@
         <v>36.349373589999999</v>
       </c>
       <c r="H15" s="11"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="50"/>
-      <c r="L15" s="50"/>
-      <c r="M15" s="50"/>
-      <c r="N15" s="50"/>
-      <c r="O15" s="50"/>
-      <c r="P15" s="50"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="49"/>
+      <c r="M15" s="49"/>
+      <c r="N15" s="49"/>
+      <c r="O15" s="49"/>
+      <c r="P15" s="49"/>
     </row>
     <row r="16" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
@@ -2091,14 +2119,14 @@
         <v>25.26471154</v>
       </c>
       <c r="H16" s="11"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="50"/>
-      <c r="K16" s="50"/>
-      <c r="L16" s="50"/>
-      <c r="M16" s="50"/>
-      <c r="N16" s="50"/>
-      <c r="O16" s="50"/>
-      <c r="P16" s="50"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="49"/>
+      <c r="L16" s="49"/>
+      <c r="M16" s="49"/>
+      <c r="N16" s="49"/>
+      <c r="O16" s="49"/>
+      <c r="P16" s="49"/>
     </row>
     <row r="17" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="18">
@@ -2123,14 +2151,14 @@
         <v>18.980193509999999</v>
       </c>
       <c r="H17" s="11"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="50"/>
-      <c r="K17" s="50"/>
-      <c r="L17" s="50"/>
-      <c r="M17" s="50"/>
-      <c r="N17" s="50"/>
-      <c r="O17" s="50"/>
-      <c r="P17" s="50"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="49"/>
+      <c r="M17" s="49"/>
+      <c r="N17" s="49"/>
+      <c r="O17" s="49"/>
+      <c r="P17" s="49"/>
     </row>
     <row r="18" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="18">
@@ -2155,14 +2183,14 @@
         <v>30.515518459999999</v>
       </c>
       <c r="H18" s="11"/>
-      <c r="I18" s="50"/>
-      <c r="J18" s="50"/>
-      <c r="K18" s="50"/>
-      <c r="L18" s="50"/>
-      <c r="M18" s="50"/>
-      <c r="N18" s="50"/>
-      <c r="O18" s="50"/>
-      <c r="P18" s="50"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="49"/>
+      <c r="M18" s="49"/>
+      <c r="N18" s="49"/>
+      <c r="O18" s="49"/>
+      <c r="P18" s="49"/>
     </row>
     <row r="19" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="18">
@@ -2187,14 +2215,14 @@
         <v>22.066696230000002</v>
       </c>
       <c r="H19" s="11"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
-      <c r="K19" s="50"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="50"/>
-      <c r="N19" s="50"/>
-      <c r="O19" s="50"/>
-      <c r="P19" s="50"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="49"/>
+      <c r="L19" s="49"/>
+      <c r="M19" s="49"/>
+      <c r="N19" s="49"/>
+      <c r="O19" s="49"/>
+      <c r="P19" s="49"/>
     </row>
     <row r="20" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="18">
@@ -2219,14 +2247,14 @@
         <v>29.31375418</v>
       </c>
       <c r="H20" s="11"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="50"/>
-      <c r="K20" s="50"/>
-      <c r="L20" s="50"/>
-      <c r="M20" s="50"/>
-      <c r="N20" s="50"/>
-      <c r="O20" s="50"/>
-      <c r="P20" s="50"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="49"/>
+      <c r="O20" s="49"/>
+      <c r="P20" s="49"/>
     </row>
     <row r="21" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
@@ -2251,14 +2279,14 @@
         <v>29.078108709999999</v>
       </c>
       <c r="H21" s="11"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="50"/>
-      <c r="K21" s="50"/>
-      <c r="L21" s="50"/>
-      <c r="M21" s="50"/>
-      <c r="N21" s="50"/>
-      <c r="O21" s="50"/>
-      <c r="P21" s="50"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="49"/>
+      <c r="N21" s="49"/>
+      <c r="O21" s="49"/>
+      <c r="P21" s="49"/>
     </row>
     <row r="22" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
@@ -2283,14 +2311,14 @@
         <v>22.563280850000002</v>
       </c>
       <c r="H22" s="11"/>
-      <c r="I22" s="50"/>
-      <c r="J22" s="50"/>
-      <c r="K22" s="50"/>
-      <c r="L22" s="50"/>
-      <c r="M22" s="50"/>
-      <c r="N22" s="50"/>
-      <c r="O22" s="50"/>
-      <c r="P22" s="50"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="49"/>
+      <c r="N22" s="49"/>
+      <c r="O22" s="49"/>
+      <c r="P22" s="49"/>
     </row>
     <row r="23" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
@@ -2315,14 +2343,14 @@
         <v>20.997673219999999</v>
       </c>
       <c r="H23" s="11"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="50"/>
-      <c r="K23" s="50"/>
-      <c r="L23" s="50"/>
-      <c r="M23" s="50"/>
-      <c r="N23" s="50"/>
-      <c r="O23" s="50"/>
-      <c r="P23" s="50"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="49"/>
+      <c r="O23" s="49"/>
+      <c r="P23" s="49"/>
     </row>
     <row r="24" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="18">
@@ -2347,14 +2375,14 @@
         <v>23.512876210000002</v>
       </c>
       <c r="H24" s="11"/>
-      <c r="I24" s="50"/>
-      <c r="J24" s="50"/>
-      <c r="K24" s="50"/>
-      <c r="L24" s="50"/>
-      <c r="M24" s="50"/>
-      <c r="N24" s="50"/>
-      <c r="O24" s="50"/>
-      <c r="P24" s="50"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="49"/>
+      <c r="N24" s="49"/>
+      <c r="O24" s="49"/>
+      <c r="P24" s="49"/>
     </row>
     <row r="25" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="29">
@@ -2366,7 +2394,7 @@
       <c r="C25" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="54" t="s">
+      <c r="D25" s="53" t="s">
         <v>8</v>
       </c>
       <c r="E25" s="22">
@@ -2379,14 +2407,14 @@
         <v>20.590849890000001</v>
       </c>
       <c r="H25" s="11"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="49"/>
-      <c r="K25" s="49"/>
-      <c r="L25" s="49"/>
-      <c r="M25" s="51"/>
-      <c r="N25" s="49"/>
-      <c r="O25" s="49"/>
-      <c r="P25" s="50"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="48"/>
+      <c r="L25" s="48"/>
+      <c r="M25" s="50"/>
+      <c r="N25" s="48"/>
+      <c r="O25" s="48"/>
+      <c r="P25" s="49"/>
     </row>
     <row r="26" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="12">
@@ -2395,7 +2423,7 @@
       <c r="B26" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="52" t="s">
+      <c r="C26" s="51" t="s">
         <v>13</v>
       </c>
       <c r="D26" s="14" t="s">
@@ -2411,14 +2439,14 @@
         <v>24.15919027</v>
       </c>
       <c r="H26" s="11"/>
-      <c r="I26" s="49"/>
-      <c r="J26" s="49"/>
-      <c r="K26" s="49"/>
-      <c r="L26" s="49"/>
-      <c r="M26" s="49"/>
-      <c r="N26" s="49"/>
-      <c r="O26" s="49"/>
-      <c r="P26" s="50"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="48"/>
+      <c r="L26" s="48"/>
+      <c r="M26" s="48"/>
+      <c r="N26" s="48"/>
+      <c r="O26" s="48"/>
+      <c r="P26" s="49"/>
     </row>
     <row r="27" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="18">
@@ -2910,7 +2938,7 @@
       <c r="B48" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C48" s="53" t="s">
+      <c r="C48" s="52" t="s">
         <v>7</v>
       </c>
       <c r="D48" s="32" t="s">
@@ -2933,4 +2961,1368 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCAE3181-10AD-FA4A-A531-0506E82FD1B0}">
+  <dimension ref="A1:G98"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="M55" sqref="M55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="45">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>73</v>
+      </c>
+      <c r="B31" s="12">
+        <v>73</v>
+      </c>
+      <c r="C31" s="40">
+        <v>73</v>
+      </c>
+      <c r="D31" s="58">
+        <v>73</v>
+      </c>
+      <c r="E31" s="58" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="61" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>74</v>
+      </c>
+      <c r="B32" s="18">
+        <v>74</v>
+      </c>
+      <c r="C32" s="40">
+        <v>74</v>
+      </c>
+      <c r="D32" s="12">
+        <v>74</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="51" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="62" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>80</v>
+      </c>
+      <c r="B33" s="18">
+        <v>80</v>
+      </c>
+      <c r="C33" s="40">
+        <v>80</v>
+      </c>
+      <c r="D33" s="18">
+        <v>80</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="54">
+        <v>84</v>
+      </c>
+      <c r="B34" s="55">
+        <v>87</v>
+      </c>
+      <c r="C34" s="40">
+        <v>87</v>
+      </c>
+      <c r="D34" s="18">
+        <v>87</v>
+      </c>
+      <c r="E34" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="64" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="54">
+        <v>85</v>
+      </c>
+      <c r="B35" s="18">
+        <v>94</v>
+      </c>
+      <c r="C35" s="40">
+        <v>94</v>
+      </c>
+      <c r="D35" s="18">
+        <v>94</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" s="25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="54">
+        <v>91</v>
+      </c>
+      <c r="B36" s="18">
+        <v>99</v>
+      </c>
+      <c r="C36" s="40">
+        <v>99</v>
+      </c>
+      <c r="D36" s="18">
+        <v>99</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" s="26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="54">
+        <v>92</v>
+      </c>
+      <c r="B37" s="55">
+        <v>103</v>
+      </c>
+      <c r="C37" s="40">
+        <v>103</v>
+      </c>
+      <c r="D37" s="18">
+        <v>103</v>
+      </c>
+      <c r="E37" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="64" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>94</v>
+      </c>
+      <c r="B38" s="18">
+        <v>199</v>
+      </c>
+      <c r="C38" s="40">
+        <v>199</v>
+      </c>
+      <c r="D38" s="18">
+        <v>199</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="54">
+        <v>97</v>
+      </c>
+      <c r="B39" s="18">
+        <v>200</v>
+      </c>
+      <c r="C39" s="40">
+        <v>200</v>
+      </c>
+      <c r="D39" s="18">
+        <v>200</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F39" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="54">
+        <v>98</v>
+      </c>
+      <c r="B40" s="18">
+        <v>201</v>
+      </c>
+      <c r="C40" s="40">
+        <v>201</v>
+      </c>
+      <c r="D40" s="18">
+        <v>201</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F40" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="54">
+        <v>99</v>
+      </c>
+      <c r="B41" s="18">
+        <v>202</v>
+      </c>
+      <c r="C41" s="40">
+        <v>202</v>
+      </c>
+      <c r="D41" s="18">
+        <v>202</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="54">
+        <v>101</v>
+      </c>
+      <c r="B42" s="18">
+        <v>203</v>
+      </c>
+      <c r="C42" s="40">
+        <v>203</v>
+      </c>
+      <c r="D42" s="18">
+        <v>203</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="54">
+        <v>107</v>
+      </c>
+      <c r="B43" s="18">
+        <v>204</v>
+      </c>
+      <c r="C43" s="40">
+        <v>204</v>
+      </c>
+      <c r="D43" s="18">
+        <v>204</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G43" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="54">
+        <v>108</v>
+      </c>
+      <c r="B44" s="18">
+        <v>205</v>
+      </c>
+      <c r="C44" s="40">
+        <v>205</v>
+      </c>
+      <c r="D44" s="18">
+        <v>205</v>
+      </c>
+      <c r="E44" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F44" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G44" s="25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="54">
+        <v>109</v>
+      </c>
+      <c r="B45" s="18">
+        <v>206</v>
+      </c>
+      <c r="C45" s="40">
+        <v>206</v>
+      </c>
+      <c r="D45" s="18">
+        <v>206</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F45" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G45" s="25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="54">
+        <v>110</v>
+      </c>
+      <c r="B46" s="18">
+        <v>207</v>
+      </c>
+      <c r="C46" s="40">
+        <v>207</v>
+      </c>
+      <c r="D46" s="18">
+        <v>207</v>
+      </c>
+      <c r="E46" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F46" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" s="25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="54">
+        <v>112</v>
+      </c>
+      <c r="B47" s="18">
+        <v>208</v>
+      </c>
+      <c r="C47" s="40">
+        <v>208</v>
+      </c>
+      <c r="D47" s="18">
+        <v>208</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F47" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" s="25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="54">
+        <v>113</v>
+      </c>
+      <c r="B48" s="18">
+        <v>209</v>
+      </c>
+      <c r="C48" s="40">
+        <v>209</v>
+      </c>
+      <c r="D48" s="18">
+        <v>209</v>
+      </c>
+      <c r="E48" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F48" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" s="25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A49" s="54">
+        <v>115</v>
+      </c>
+      <c r="B49" s="18">
+        <v>210</v>
+      </c>
+      <c r="C49" s="40">
+        <v>210</v>
+      </c>
+      <c r="D49" s="18">
+        <v>210</v>
+      </c>
+      <c r="E49" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G49" s="25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" s="54">
+        <v>116</v>
+      </c>
+      <c r="B50" s="18">
+        <v>211</v>
+      </c>
+      <c r="C50" s="40">
+        <v>211</v>
+      </c>
+      <c r="D50" s="18">
+        <v>211</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F50" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G50" s="26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51" s="54">
+        <v>117</v>
+      </c>
+      <c r="B51" s="18">
+        <v>212</v>
+      </c>
+      <c r="C51" s="40">
+        <v>212</v>
+      </c>
+      <c r="D51" s="18">
+        <v>212</v>
+      </c>
+      <c r="E51" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F51" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G51" s="26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="54">
+        <v>118</v>
+      </c>
+      <c r="B52" s="18">
+        <v>213</v>
+      </c>
+      <c r="C52" s="40">
+        <v>213</v>
+      </c>
+      <c r="D52" s="18">
+        <v>213</v>
+      </c>
+      <c r="E52" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F52" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G52" s="26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53" s="54">
+        <v>124</v>
+      </c>
+      <c r="B53" s="55">
+        <v>214</v>
+      </c>
+      <c r="C53" s="42">
+        <v>214</v>
+      </c>
+      <c r="D53" s="18">
+        <v>214</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F53" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G53" s="64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="54">
+        <v>125</v>
+      </c>
+      <c r="B54" s="56">
+        <v>215</v>
+      </c>
+      <c r="C54" s="45">
+        <v>215</v>
+      </c>
+      <c r="D54" s="18">
+        <v>215</v>
+      </c>
+      <c r="E54" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F54" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G54" s="64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="54">
+        <v>126</v>
+      </c>
+      <c r="B55" s="57">
+        <v>216</v>
+      </c>
+      <c r="C55" s="40">
+        <v>216</v>
+      </c>
+      <c r="D55" s="29">
+        <v>216</v>
+      </c>
+      <c r="E55" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="F55" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="G55" s="65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="54">
+        <v>127</v>
+      </c>
+      <c r="B56" s="55">
+        <v>217</v>
+      </c>
+      <c r="D56" s="12">
+        <v>217</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F56" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" s="66" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A57" s="54">
+        <v>128</v>
+      </c>
+      <c r="B57" s="55">
+        <v>218</v>
+      </c>
+      <c r="C57" s="40">
+        <v>218</v>
+      </c>
+      <c r="D57" s="18">
+        <v>218</v>
+      </c>
+      <c r="E57" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F57" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G57" s="64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="54">
+        <v>129</v>
+      </c>
+      <c r="B58" s="55">
+        <v>219</v>
+      </c>
+      <c r="C58" s="40">
+        <v>219</v>
+      </c>
+      <c r="D58" s="18">
+        <v>219</v>
+      </c>
+      <c r="E58" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F58" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G58" s="64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="54">
+        <v>131</v>
+      </c>
+      <c r="B59" s="18">
+        <v>220</v>
+      </c>
+      <c r="C59" s="40">
+        <v>220</v>
+      </c>
+      <c r="D59" s="18">
+        <v>220</v>
+      </c>
+      <c r="E59" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G59" s="26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="54">
+        <v>136</v>
+      </c>
+      <c r="B60" s="18">
+        <v>301</v>
+      </c>
+      <c r="C60" s="40">
+        <v>301</v>
+      </c>
+      <c r="D60" s="18">
+        <v>301</v>
+      </c>
+      <c r="E60" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G60" s="26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="54">
+        <v>137</v>
+      </c>
+      <c r="B61" s="18">
+        <v>302</v>
+      </c>
+      <c r="C61" s="40">
+        <v>302</v>
+      </c>
+      <c r="D61" s="18">
+        <v>302</v>
+      </c>
+      <c r="E61" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G61" s="26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="54">
+        <v>138</v>
+      </c>
+      <c r="B62" s="18">
+        <v>303</v>
+      </c>
+      <c r="C62" s="40">
+        <v>303</v>
+      </c>
+      <c r="D62" s="18">
+        <v>303</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G62" s="25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="54">
+        <v>139</v>
+      </c>
+      <c r="B63" s="18">
+        <v>304</v>
+      </c>
+      <c r="C63" s="40">
+        <v>304</v>
+      </c>
+      <c r="D63" s="18">
+        <v>304</v>
+      </c>
+      <c r="E63" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G63" s="64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="54">
+        <v>140</v>
+      </c>
+      <c r="B64" s="18">
+        <v>305</v>
+      </c>
+      <c r="C64" s="40">
+        <v>305</v>
+      </c>
+      <c r="D64" s="18">
+        <v>305</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G64" s="25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A65" s="54">
+        <v>141</v>
+      </c>
+      <c r="B65" s="18">
+        <v>306</v>
+      </c>
+      <c r="C65" s="40">
+        <v>306</v>
+      </c>
+      <c r="D65" s="18">
+        <v>306</v>
+      </c>
+      <c r="E65" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G65" s="26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A66" s="54">
+        <v>142</v>
+      </c>
+      <c r="B66" s="18">
+        <v>307</v>
+      </c>
+      <c r="C66" s="40">
+        <v>307</v>
+      </c>
+      <c r="D66" s="18">
+        <v>307</v>
+      </c>
+      <c r="E66" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G66" s="26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="54">
+        <v>143</v>
+      </c>
+      <c r="B67" s="18">
+        <v>308</v>
+      </c>
+      <c r="C67" s="40">
+        <v>308</v>
+      </c>
+      <c r="D67" s="18">
+        <v>308</v>
+      </c>
+      <c r="E67" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G67" s="25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A68" s="54">
+        <v>144</v>
+      </c>
+      <c r="B68" s="18">
+        <v>309</v>
+      </c>
+      <c r="C68" s="40">
+        <v>309</v>
+      </c>
+      <c r="D68" s="18">
+        <v>309</v>
+      </c>
+      <c r="E68" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G68" s="25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A69" s="54">
+        <v>145</v>
+      </c>
+      <c r="B69" s="55">
+        <v>310</v>
+      </c>
+      <c r="C69" s="40">
+        <v>310</v>
+      </c>
+      <c r="D69" s="18">
+        <v>310</v>
+      </c>
+      <c r="E69" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G69" s="64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A70" s="54">
+        <v>146</v>
+      </c>
+      <c r="B70" s="55">
+        <v>311</v>
+      </c>
+      <c r="C70" s="40">
+        <v>311</v>
+      </c>
+      <c r="D70" s="18">
+        <v>311</v>
+      </c>
+      <c r="E70" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G70" s="64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A71" s="54">
+        <v>147</v>
+      </c>
+      <c r="B71" s="55">
+        <v>312</v>
+      </c>
+      <c r="C71" s="40">
+        <v>312</v>
+      </c>
+      <c r="D71" s="18">
+        <v>312</v>
+      </c>
+      <c r="E71" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="F71" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G71" s="64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A72" s="54">
+        <v>198</v>
+      </c>
+      <c r="B72" s="55">
+        <v>313</v>
+      </c>
+      <c r="C72" s="40">
+        <v>313</v>
+      </c>
+      <c r="D72" s="18">
+        <v>313</v>
+      </c>
+      <c r="E72" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G72" s="64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>199</v>
+      </c>
+      <c r="B73" s="55">
+        <v>314</v>
+      </c>
+      <c r="C73" s="40">
+        <v>314</v>
+      </c>
+      <c r="D73" s="18">
+        <v>314</v>
+      </c>
+      <c r="E73" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="F73" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G73" s="64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>200</v>
+      </c>
+      <c r="B74" s="55">
+        <v>315</v>
+      </c>
+      <c r="C74" s="40">
+        <v>315</v>
+      </c>
+      <c r="D74" s="18">
+        <v>315</v>
+      </c>
+      <c r="E74" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G74" s="64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>201</v>
+      </c>
+      <c r="B75" s="55">
+        <v>316</v>
+      </c>
+      <c r="C75" s="40">
+        <v>316</v>
+      </c>
+      <c r="D75" s="18">
+        <v>316</v>
+      </c>
+      <c r="E75" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="F75" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G75" s="64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>202</v>
+      </c>
+      <c r="B76" s="18">
+        <v>317</v>
+      </c>
+      <c r="C76" s="40">
+        <v>317</v>
+      </c>
+      <c r="D76" s="18">
+        <v>317</v>
+      </c>
+      <c r="E76" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F76" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G76" s="26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>203</v>
+      </c>
+      <c r="B77" s="29">
+        <v>318</v>
+      </c>
+      <c r="C77" s="42">
+        <v>318</v>
+      </c>
+      <c r="D77" s="18">
+        <v>318</v>
+      </c>
+      <c r="E77" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F77" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G77" s="26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>204</v>
+      </c>
+      <c r="D78" s="42"/>
+      <c r="E78" s="43"/>
+      <c r="F78" s="43"/>
+      <c r="G78" s="43"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>318</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D31:G78">
+    <sortCondition ref="D31:D78"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>